<commit_message>
Added chapter to lit review, updated final pdf, updated totals.xlsx
</commit_message>
<xml_diff>
--- a/Results/Totals.xlsx
+++ b/Results/Totals.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TuDublin\Masters Project\Git Clone\MastersProject2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TuDublin\Masters Project\Git Clone\MastersProject2021\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06BDA79-3730-4D27-95D1-931FC8F307E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7102D8EC-DA17-46DE-854A-20B35ED4E5C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A673DB8F-DC50-4B7A-BE4B-35EE518A0E19}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>AssemblyScript</t>
   </si>
@@ -78,13 +78,25 @@
   </si>
   <si>
     <t>BubbleSort</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>2nd</t>
+  </si>
+  <si>
+    <t>3rd</t>
+  </si>
+  <si>
+    <t>4th</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,16 +112,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -118,10 +149,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -131,8 +162,71 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -142,97 +236,68 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -241,19 +306,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,241 +642,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0422ED53-8CB1-47FA-8151-F82FFD842153}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="21" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="6" width="21" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="2:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" s="13" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5">
+      <c r="C4" s="6">
+        <v>813.92754360000004</v>
+      </c>
+      <c r="D4" s="6">
+        <v>832.37303689999999</v>
+      </c>
+      <c r="E4" s="6">
+        <v>747.50733590000004</v>
+      </c>
+      <c r="F4" s="1">
         <v>1028.4816080000001</v>
       </c>
-      <c r="C2" s="5">
-        <v>832.37303689999999</v>
-      </c>
-      <c r="D2" s="5">
-        <v>813.92754360000004</v>
-      </c>
-      <c r="E2" s="6">
-        <v>747.50733590000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5">
+      <c r="C5" s="6">
+        <v>59.14979537</v>
+      </c>
+      <c r="D5" s="6">
+        <v>58.054743279999997</v>
+      </c>
+      <c r="E5" s="6">
+        <v>112.3503863</v>
+      </c>
+      <c r="F5" s="1">
         <v>547.56293860000005</v>
       </c>
-      <c r="C3" s="5">
-        <v>58.054743279999997</v>
-      </c>
-      <c r="D3" s="5">
-        <v>59.14979537</v>
-      </c>
-      <c r="E3" s="6">
-        <v>112.3503863</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
+      <c r="C6" s="6">
+        <v>36.501139930000001</v>
+      </c>
+      <c r="D6" s="6">
+        <v>43.554516360000001</v>
+      </c>
+      <c r="E6" s="6">
+        <v>45.262973729999999</v>
+      </c>
+      <c r="F6" s="1">
         <v>376.1207794</v>
       </c>
-      <c r="C4" s="5">
-        <v>43.554516360000001</v>
-      </c>
-      <c r="D4" s="5">
-        <v>36.501139930000001</v>
-      </c>
-      <c r="E4" s="6">
-        <v>45.262973729999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
+      <c r="C7" s="6">
+        <v>50.410140820000002</v>
+      </c>
+      <c r="D7" s="6">
+        <v>58.152907380000002</v>
+      </c>
+      <c r="E7" s="6">
+        <v>63.607786650000001</v>
+      </c>
+      <c r="F7" s="1">
         <v>517.36718819999999</v>
       </c>
-      <c r="C5" s="5">
-        <v>58.152907380000002</v>
-      </c>
-      <c r="D5" s="5">
-        <v>50.410140820000002</v>
-      </c>
-      <c r="E5" s="6">
-        <v>63.607786650000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
+      <c r="C8" s="6">
+        <v>3.6349287850000001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>3.55388708</v>
+      </c>
+      <c r="E8" s="6">
+        <v>2.9489402849999999</v>
+      </c>
+      <c r="F8" s="1">
         <v>4.7098711099999999</v>
       </c>
-      <c r="C6" s="5">
-        <v>3.55388708</v>
-      </c>
-      <c r="D6" s="5">
-        <v>3.6349287850000001</v>
-      </c>
-      <c r="E6" s="6">
-        <v>2.9489402849999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5">
+      <c r="C9" s="6">
+        <v>653.96304450000002</v>
+      </c>
+      <c r="D9" s="6">
+        <v>673.32442319999996</v>
+      </c>
+      <c r="E9" s="6">
+        <v>432.8657695</v>
+      </c>
+      <c r="F9" s="1">
         <v>1627.994193</v>
       </c>
-      <c r="C7" s="5">
-        <v>673.32442319999996</v>
-      </c>
-      <c r="D7" s="5">
-        <v>653.96304450000002</v>
-      </c>
-      <c r="E7" s="6">
-        <v>432.8657695</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
+      <c r="C10" s="6">
+        <v>2.2011099399999998</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2.1928160069999998</v>
+      </c>
+      <c r="E10" s="6">
+        <v>3.6119719269999999</v>
+      </c>
+      <c r="F10" s="1">
         <v>14.57914214</v>
       </c>
-      <c r="C8" s="5">
-        <v>2.1928160069999998</v>
-      </c>
-      <c r="D8" s="5">
-        <v>2.2011099399999998</v>
-      </c>
-      <c r="E8" s="6">
-        <v>3.6119719269999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5">
+      <c r="C11" s="6">
+        <v>1.44226305</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.411856896</v>
+      </c>
+      <c r="E11" s="6">
+        <v>9.8547817470000005</v>
+      </c>
+      <c r="F11" s="1">
         <v>6.7146736760000003</v>
       </c>
-      <c r="C9" s="5">
-        <v>1.411856896</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1.44226305</v>
-      </c>
-      <c r="E9" s="6">
-        <v>9.8547817470000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5">
+      <c r="C12" s="6">
+        <v>1.071705701</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.047660574</v>
+      </c>
+      <c r="E12" s="6">
+        <v>2.8299523290000002</v>
+      </c>
+      <c r="F12" s="1">
         <v>3.4219469579999999</v>
       </c>
-      <c r="C10" s="5">
-        <v>1.047660574</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1.071705701</v>
-      </c>
-      <c r="E10" s="6">
-        <v>2.8299523290000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5">
+      <c r="C13" s="6">
+        <v>486.01185470000001</v>
+      </c>
+      <c r="D13" s="6">
+        <v>499.6437487</v>
+      </c>
+      <c r="E13" s="6">
+        <v>885.54548199999999</v>
+      </c>
+      <c r="F13" s="1">
         <v>3864.9485719999998</v>
       </c>
-      <c r="C11" s="5">
-        <v>499.6437487</v>
-      </c>
-      <c r="D11" s="5">
-        <v>486.01185470000001</v>
-      </c>
-      <c r="E11" s="6">
-        <v>885.54548199999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="5">
+      <c r="C14" s="6">
+        <v>943.48911869999995</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1010.069966</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1158.0128239999999</v>
+      </c>
+      <c r="F14" s="10">
         <v>8793.6478200000001</v>
       </c>
-      <c r="C12" s="5">
-        <v>1010.069966</v>
-      </c>
-      <c r="D12" s="5">
-        <v>943.48911869999995</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1158.0128239999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10">
-        <f>SUM(B2:B12)</f>
+    </row>
+    <row r="15" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="9"/>
+      <c r="C15" s="7">
+        <f>SUM(C4:C14)</f>
+        <v>3051.8026450960001</v>
+      </c>
+      <c r="D15" s="7">
+        <f>SUM(D4:D14)</f>
+        <v>3183.3795623769997</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" ref="E15" si="0">SUM(E4:E14)</f>
+        <v>3464.3982043680003</v>
+      </c>
+      <c r="F15" s="2">
+        <f>SUM(F4:F14)</f>
         <v>16785.548733084001</v>
       </c>
-      <c r="C13" s="10">
-        <f t="shared" ref="C13:E13" si="0">SUM(C2:C12)</f>
-        <v>3183.3795623769997</v>
-      </c>
-      <c r="D13" s="10">
-        <f t="shared" si="0"/>
-        <v>3051.8026450960001</v>
-      </c>
-      <c r="E13" s="11">
-        <f t="shared" si="0"/>
-        <v>3464.3982043680003</v>
-      </c>
-    </row>
+    </row>
+    <row r="16" spans="2:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="B13:E13">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="C15:F15">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>